<commit_message>
Actualización sidebar, generación clave
-Nueva ruta en sidebar
-Conexión de la generación de claves a la base de datos
</commit_message>
<xml_diff>
--- a/my-app/static/downloads-excel/Reporte_empleados_2023_11_27.xlsx
+++ b/my-app/static/downloads-excel/Reporte_empleados_2023_11_27.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -456,17 +456,17 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>45254</v>
+        <v>45257.41307870371</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1234</t>
+          <t>Nyw5LR</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -474,45 +474,99 @@
         </is>
       </c>
       <c r="C3" s="1" t="n">
-        <v>45253</v>
+        <v>45257.41237268518</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1234</t>
+          <t>111</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0123456789</t>
+          <t>0105781496</t>
         </is>
       </c>
       <c r="C4" s="1" t="n">
-        <v>45251</v>
+        <v>45257</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>111</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0105781496</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>45254</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0105781496</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>45253</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0123456789</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>45251</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>2</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>0123456789</t>
         </is>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C8" s="1" t="n">
         <v>45250</v>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>123</t>
         </is>

</xml_diff>

<commit_message>
usuarios, docker y conexiones
-Gestion de usuarios por parte del administrador
-Creacion de dockerfile
</commit_message>
<xml_diff>
--- a/my-app/static/downloads-excel/Reporte_empleados_2023_11_27.xlsx
+++ b/my-app/static/downloads-excel/Reporte_empleados_2023_11_27.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -456,17 +456,17 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>45257.41307870371</v>
+        <v>45257.83576388889</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Nyw5LR</t>
+          <t>SwR2Wh</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -474,17 +474,17 @@
         </is>
       </c>
       <c r="C3" s="1" t="n">
-        <v>45257.41237268518</v>
+        <v>45257.41307870371</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>111</t>
+          <t>Nyw5LR</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" s="1" t="n">
-        <v>45257</v>
+        <v>45257.41237268518</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -502,7 +502,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -510,17 +510,17 @@
         </is>
       </c>
       <c r="C5" s="1" t="n">
-        <v>45254</v>
+        <v>45257</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1234</t>
+          <t>111</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -528,7 +528,7 @@
         </is>
       </c>
       <c r="C6" s="1" t="n">
-        <v>45253</v>
+        <v>45254</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -538,35 +538,71 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0123456789</t>
+          <t>0105781496</t>
         </is>
       </c>
       <c r="C7" s="1" t="n">
-        <v>45251</v>
+        <v>45253</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>1234</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
+        <v>9</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0123456789</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>45257.83667824074</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>3D9AlD</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0123456789</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>45251</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>2</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>0123456789</t>
         </is>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C10" s="1" t="n">
         <v>45250</v>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>123</t>
         </is>

</xml_diff>